<commit_message>
Updated: Pins of RunStop & Step(RotEnc)
</commit_message>
<xml_diff>
--- a/ベースマシン UI Controller 接続一覧表.xlsx
+++ b/ベースマシン UI Controller 接続一覧表.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="147">
   <si>
     <t>VCO</t>
     <phoneticPr fontId="1"/>
@@ -377,10 +377,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>PB_9, PB_8</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>PA_0</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -590,10 +586,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>PA_12</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>RESET</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -607,6 +599,18 @@
   </si>
   <si>
     <t>SCK</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>PA_11, PA_12</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>PB_9</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>D14</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1108,7 +1112,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
@@ -1129,7 +1133,7 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -1157,11 +1161,11 @@
         <v>32</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H5" s="10"/>
       <c r="I5" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -1182,7 +1186,7 @@
       </c>
       <c r="G6" s="8"/>
       <c r="I6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -1196,11 +1200,11 @@
         <v>28</v>
       </c>
       <c r="F7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G7" s="6"/>
       <c r="I7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -1220,11 +1224,11 @@
         <v>37</v>
       </c>
       <c r="F8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G8" s="4"/>
       <c r="I8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -1241,11 +1245,11 @@
         <v>38</v>
       </c>
       <c r="F9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G9" s="3"/>
       <c r="I9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -1259,11 +1263,11 @@
         <v>28</v>
       </c>
       <c r="F10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G10" s="8"/>
       <c r="I10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -1280,14 +1284,14 @@
         <v>28</v>
       </c>
       <c r="E11" t="s">
+        <v>91</v>
+      </c>
+      <c r="F11" t="s">
         <v>92</v>
-      </c>
-      <c r="F11" t="s">
-        <v>93</v>
       </c>
       <c r="G11" s="5"/>
       <c r="I11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -1307,11 +1311,11 @@
         <v>34</v>
       </c>
       <c r="F12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G12" s="11"/>
       <c r="I12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -1328,11 +1332,11 @@
         <v>35</v>
       </c>
       <c r="F13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G13" s="13"/>
       <c r="I13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -1349,11 +1353,11 @@
         <v>36</v>
       </c>
       <c r="F14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G14" s="12"/>
       <c r="I14" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -1373,12 +1377,12 @@
         <v>54</v>
       </c>
       <c r="F15" t="s">
-        <v>86</v>
+        <v>144</v>
       </c>
       <c r="G15" s="4"/>
       <c r="H15" s="11"/>
       <c r="I15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -1400,7 +1404,7 @@
       <c r="G16" s="13"/>
       <c r="H16" s="12"/>
       <c r="I16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -1414,15 +1418,15 @@
         <v>30</v>
       </c>
       <c r="E17" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F17" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G17" s="11"/>
       <c r="H17" s="4"/>
       <c r="I17" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -1436,11 +1440,11 @@
         <v>29</v>
       </c>
       <c r="F18" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G18" s="16"/>
       <c r="I18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -1454,11 +1458,11 @@
         <v>29</v>
       </c>
       <c r="F19" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G19" s="14"/>
       <c r="I19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -1472,11 +1476,11 @@
         <v>29</v>
       </c>
       <c r="F20" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G20" s="12"/>
       <c r="I20" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -1494,144 +1498,144 @@
       </c>
       <c r="G21" s="13"/>
       <c r="I21" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B22" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C22" t="s">
+        <v>124</v>
+      </c>
+      <c r="D22" t="s">
         <v>125</v>
       </c>
-      <c r="D22" t="s">
+      <c r="F22" t="s">
         <v>126</v>
-      </c>
-      <c r="F22" t="s">
-        <v>127</v>
       </c>
       <c r="G22" s="12"/>
     </row>
     <row r="23" spans="1:9">
       <c r="B23" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C23" t="s">
+        <v>124</v>
+      </c>
+      <c r="D23" t="s">
         <v>125</v>
       </c>
-      <c r="D23" t="s">
-        <v>126</v>
-      </c>
       <c r="F23" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G23" s="13"/>
     </row>
     <row r="24" spans="1:9">
       <c r="B24" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C24" t="s">
+        <v>124</v>
+      </c>
+      <c r="D24" t="s">
         <v>125</v>
       </c>
-      <c r="D24" t="s">
-        <v>126</v>
-      </c>
       <c r="F24" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G24" s="11"/>
     </row>
     <row r="25" spans="1:9">
       <c r="B25" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C25" t="s">
+        <v>124</v>
+      </c>
+      <c r="D25" t="s">
         <v>125</v>
       </c>
-      <c r="D25" t="s">
-        <v>126</v>
-      </c>
       <c r="F25" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G25" s="4"/>
     </row>
     <row r="26" spans="1:9">
       <c r="B26" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C26" t="s">
+        <v>124</v>
+      </c>
+      <c r="D26" t="s">
         <v>125</v>
       </c>
-      <c r="D26" t="s">
-        <v>126</v>
-      </c>
       <c r="F26" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G26" s="3"/>
     </row>
     <row r="27" spans="1:9">
       <c r="B27" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C27" t="s">
+        <v>124</v>
+      </c>
+      <c r="D27" t="s">
         <v>125</v>
       </c>
-      <c r="D27" t="s">
-        <v>126</v>
-      </c>
       <c r="E27" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F27" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G27" s="5"/>
     </row>
     <row r="28" spans="1:9">
       <c r="B28" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C28" t="s">
+        <v>124</v>
+      </c>
+      <c r="D28" t="s">
         <v>125</v>
       </c>
-      <c r="D28" t="s">
-        <v>126</v>
-      </c>
       <c r="E28" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F28" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G28" s="6"/>
     </row>
     <row r="29" spans="1:9">
       <c r="B29" t="s">
+        <v>123</v>
+      </c>
+      <c r="C29" t="s">
         <v>124</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>125</v>
       </c>
-      <c r="D29" t="s">
-        <v>126</v>
-      </c>
       <c r="E29" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F29" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G29" s="15"/>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B30" t="s">
         <v>20</v>
@@ -1643,52 +1647,52 @@
         <v>30</v>
       </c>
       <c r="F30" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G30" s="5"/>
       <c r="H30" s="6"/>
       <c r="I30" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="31" spans="1:9">
       <c r="B31" t="s">
+        <v>101</v>
+      </c>
+      <c r="C31" t="s">
         <v>102</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>103</v>
       </c>
-      <c r="D31" t="s">
+      <c r="F31" t="s">
         <v>104</v>
-      </c>
-      <c r="F31" t="s">
-        <v>105</v>
       </c>
       <c r="G31" s="18"/>
       <c r="H31" s="7"/>
       <c r="I31" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="32" spans="1:9">
       <c r="B32" t="s">
+        <v>97</v>
+      </c>
+      <c r="C32" t="s">
         <v>98</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>99</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
+        <v>97</v>
+      </c>
+      <c r="F32" t="s">
         <v>100</v>
-      </c>
-      <c r="E32" t="s">
-        <v>98</v>
-      </c>
-      <c r="F32" t="s">
-        <v>101</v>
       </c>
       <c r="G32" s="3"/>
       <c r="I32" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="34" spans="1:9">
@@ -1716,22 +1720,22 @@
         <v>32</v>
       </c>
       <c r="G35" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H35" s="10"/>
       <c r="I35" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="36" spans="1:9">
       <c r="A36" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B36" t="s">
         <v>43</v>
       </c>
       <c r="C36" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D36" t="s">
         <v>29</v>
@@ -1741,7 +1745,7 @@
       </c>
       <c r="G36" s="8"/>
       <c r="I36" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="37" spans="1:9">
@@ -1756,7 +1760,7 @@
       </c>
       <c r="G37" s="6"/>
       <c r="I37" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="38" spans="1:9">
@@ -1771,7 +1775,7 @@
       </c>
       <c r="G38" s="11"/>
       <c r="I38" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="39" spans="1:9">
@@ -1786,7 +1790,7 @@
       </c>
       <c r="G39" s="13"/>
       <c r="I39" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="40" spans="1:9">
@@ -1801,7 +1805,7 @@
       </c>
       <c r="G40" s="12"/>
       <c r="I40" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="42" spans="1:9">
@@ -1829,11 +1833,11 @@
         <v>32</v>
       </c>
       <c r="G43" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H43" s="10"/>
       <c r="I43" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="44" spans="1:9">
@@ -1849,7 +1853,7 @@
         <v>66</v>
       </c>
       <c r="I44" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="45" spans="1:9">
@@ -1863,7 +1867,7 @@
         <v>67</v>
       </c>
       <c r="I45" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="46" spans="1:9">
@@ -1877,7 +1881,7 @@
         <v>68</v>
       </c>
       <c r="I46" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="47" spans="1:9">
@@ -1888,7 +1892,7 @@
         <v>71</v>
       </c>
       <c r="C47" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D47" t="s">
         <v>59</v>
@@ -1901,7 +1905,7 @@
       </c>
       <c r="G47" s="4"/>
       <c r="I47" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="48" spans="1:9">
@@ -1922,7 +1926,7 @@
       </c>
       <c r="G48" s="11"/>
       <c r="I48" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="49" spans="1:9">
@@ -1943,7 +1947,7 @@
       </c>
       <c r="G49" s="3"/>
       <c r="I49" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="50" spans="1:9">
@@ -1964,7 +1968,7 @@
       </c>
       <c r="G50" s="16"/>
       <c r="I50" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="51" spans="1:9">
@@ -1972,7 +1976,7 @@
         <v>71</v>
       </c>
       <c r="C51" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D51" t="s">
         <v>59</v>
@@ -1985,27 +1989,30 @@
       </c>
       <c r="G51" s="17"/>
       <c r="I51" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="52" spans="1:9">
       <c r="B52" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D52" t="s">
-        <v>126</v>
+        <v>125</v>
+      </c>
+      <c r="E52" t="s">
+        <v>146</v>
       </c>
       <c r="F52" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="G52" s="19"/>
       <c r="I52" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="53" spans="1:9">
       <c r="A53" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B53" t="s">
         <v>72</v>
@@ -2024,7 +2031,7 @@
       </c>
       <c r="G53" s="7"/>
       <c r="I53" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="54" spans="1:9">
@@ -2044,7 +2051,7 @@
         <v>78</v>
       </c>
       <c r="I54" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>